<commit_message>
Cleaned up formatting, added citation
</commit_message>
<xml_diff>
--- a/Data/03_ProportionData/USIndustryEmploymentData2016.xlsx
+++ b/Data/03_ProportionData/USIndustryEmploymentData2016.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JeffThompson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JeffThompson/Documents/DataVisualization/Data/03_ProportionData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="500" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="40740" yWindow="460" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="320">
   <si>
     <t>Total employed</t>
   </si>
@@ -978,6 +978,15 @@
   </si>
   <si>
     <t>https://www.bls.gov/cps/lfcharacteristics.htm#occind</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>US Bureau of Labor Statistics</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
   </si>
 </sst>
 </file>
@@ -986,9 +995,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1007,9 +1016,37 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1029,42 +1066,53 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1340,2539 +1388,2560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B331"/>
+  <dimension ref="A2:B335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="52" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="8" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B9" s="2">
         <v>151436000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="11" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="12" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B12" s="2">
         <v>2460000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="13" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B13" s="2">
         <v>1206000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="14" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B14" s="2">
         <v>876000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="15" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B15" s="2">
         <v>58000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="16" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B16" s="2">
         <v>101000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="17" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B17" s="2">
         <v>38000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="18" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B18" s="2">
         <v>180000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+    <row r="20" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B20" s="2">
         <v>792000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="21" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B21" s="2">
         <v>102000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="22" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B22" s="2">
         <v>53000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="23" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B23" s="2">
         <v>37000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="24" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B24" s="2">
         <v>106000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="25" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B25" s="2">
         <v>6000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="26" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B26" s="2">
         <v>488000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+    <row r="28" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B28" s="2">
         <v>10328000</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    <row r="30" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B30" s="2">
         <v>15408000</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="31" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B31" s="2">
         <v>9704000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="32" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B32" s="2">
         <v>450000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+    <row r="33" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B33" s="2">
         <v>28000</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+    <row r="34" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B34" s="2">
         <v>20000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+    <row r="35" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B35" s="2">
         <v>162000</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+    <row r="36" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B36" s="2">
         <v>149000</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+    <row r="37" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B37" s="2">
         <v>92000</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="38" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B38" s="2">
         <v>1632000</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+    <row r="39" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B39" s="2">
         <v>269000</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+    <row r="40" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B40" s="2">
         <v>72000</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+    <row r="41" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B41" s="2">
         <v>44000</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+    <row r="42" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B42" s="2">
         <v>72000</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+    <row r="43" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B43" s="2">
         <v>48000</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+    <row r="44" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B44" s="2">
         <v>43000</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+    <row r="45" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B45" s="2">
         <v>336000</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+    <row r="46" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B46" s="2">
         <v>306000</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+    <row r="47" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B47" s="2">
         <v>76000</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="48" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B48" s="2">
         <v>50000</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+    <row r="49" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B49" s="2">
         <v>292000</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+    <row r="50" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B50" s="2">
         <v>26000</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="51" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B51" s="2">
         <v>1186000</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="52" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B52" s="2">
         <v>110000</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+    <row r="53" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B53" s="2">
         <v>156000</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+    <row r="54" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B54" s="2">
         <v>72000</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+    <row r="55" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B55" s="2">
         <v>145000</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+    <row r="56" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B56" s="2">
         <v>58000</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+    <row r="57" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B57" s="2">
         <v>634000</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+    <row r="58" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B58" s="2">
         <v>12000</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+    <row r="59" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B59" s="2">
         <v>1215000</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+    <row r="60" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B60" s="2">
         <v>196000</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+    <row r="61" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B61" s="2">
         <v>152000</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+    <row r="62" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B62" s="2">
         <v>218000</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+    <row r="63" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B63" s="2">
         <v>650000</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+    <row r="64" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B64" s="2">
         <v>387000</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+    <row r="65" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B65" s="2">
         <v>75000</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+    <row r="66" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B66" s="2">
         <v>312000</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+    <row r="67" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B67" s="2">
         <v>2438000</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+    <row r="68" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B68" s="2">
         <v>1401000</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+    <row r="69" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B69" s="2">
         <v>729000</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+    <row r="70" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B70" s="2">
         <v>73000</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+    <row r="71" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B71" s="2">
         <v>23000</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+    <row r="72" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B72" s="2">
         <v>174000</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+    <row r="73" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B73" s="2">
         <v>38000</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="74" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B74" s="2">
         <v>419000</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+    <row r="75" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B75" s="2">
         <v>111000</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+    <row r="76" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B76" s="2">
         <v>38000</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+    <row r="77" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B77" s="2">
         <v>42000</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+    <row r="78" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B78" s="2">
         <v>228000</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="79" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B79" s="2">
         <v>441000</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="80" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B80" s="2">
         <v>1536000</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+    <row r="81" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B81" s="2">
         <v>585000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+    <row r="82" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B82" s="2">
         <v>97000</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+    <row r="83" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B83" s="2">
         <v>556000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+    <row r="84" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B84" s="2">
         <v>297000</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+    <row r="85" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B85" s="2">
         <v>5704000</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="86" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B86" s="2">
         <v>1770000</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+    <row r="87" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B87" s="2">
         <v>142000</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+    <row r="88" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B88" s="2">
         <v>80000</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+    <row r="89" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B89" s="2">
         <v>157000</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
+    <row r="90" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B90" s="2">
         <v>132000</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+    <row r="91" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B91" s="2">
         <v>481000</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+    <row r="92" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B92" s="2">
         <v>298000</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+    <row r="93" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B93" s="2">
         <v>217000</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
+    <row r="94" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B94" s="2">
         <v>216000</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
+    <row r="95" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B95" s="2">
         <v>48000</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+    <row r="96" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B96" s="2">
         <v>323000</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+    <row r="97" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B97" s="2">
         <v>304000</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+    <row r="98" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B98" s="2">
         <v>19000</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+    <row r="99" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B99" s="2">
         <v>643000</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
+    <row r="100" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B100" s="2">
         <v>9000</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+    <row r="101" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B101" s="2">
         <v>105000</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+    <row r="102" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B102" s="2">
         <v>22000</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
+    <row r="103" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B103" s="2">
         <v>76000</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+    <row r="104" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B104" s="2">
         <v>89000</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
+    <row r="105" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B105" s="2">
         <v>21000</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+    <row r="106" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B106" s="2">
         <v>253000</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
+    <row r="107" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B107" s="2">
         <v>5000</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="5" t="s">
+    <row r="108" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B108" s="2">
         <v>42000</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+    <row r="109" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B109" s="2">
         <v>21000</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+    <row r="110" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B110" s="2">
         <v>909000</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
+    <row r="111" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B111" s="2">
         <v>203000</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
+    <row r="112" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B112" s="2">
         <v>109000</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
+    <row r="113" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B113" s="2">
         <v>85000</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+    <row r="114" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B114" s="2">
         <v>511000</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+    <row r="115" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B115" s="2">
         <v>179000</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
+    <row r="116" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B116" s="2">
         <v>167000</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
+    <row r="117" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B117" s="2">
         <v>12000</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+    <row r="118" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B118" s="2">
         <v>1323000</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+    <row r="119" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B119" s="2">
         <v>127000</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="5" t="s">
+    <row r="120" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B120" s="2">
         <v>35000</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="5" t="s">
+    <row r="121" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B121" s="2">
         <v>556000</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="5" t="s">
+    <row r="122" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B122" s="2">
         <v>70000</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A119" s="5" t="s">
+    <row r="123" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B123" s="2">
         <v>134000</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="5" t="s">
+    <row r="124" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B124" s="2">
         <v>401000</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
+    <row r="125" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B125" s="2">
         <v>556000</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="5" t="s">
+    <row r="126" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B126" s="2">
         <v>407000</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="5" t="s">
+    <row r="127" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B123" s="6">
+      <c r="B127" s="2">
         <v>65000</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+    <row r="128" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B128" s="2">
         <v>83000</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="9" t="s">
+    <row r="130" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B130" s="2">
         <v>20218000</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
+    <row r="131" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B131" s="2">
         <v>3641000</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
+    <row r="132" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B132" s="2">
         <v>193000</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
+    <row r="133" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B133" s="2">
         <v>67000</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
+    <row r="134" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B134" s="2">
         <v>171000</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+    <row r="135" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B135" s="2">
         <v>320000</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
+    <row r="136" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B136" s="2">
         <v>52000</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
+    <row r="137" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B137" s="2">
         <v>180000</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
+    <row r="138" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B138" s="2">
         <v>164000</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
+    <row r="139" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B139" s="2">
         <v>371000</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
+    <row r="140" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B140" s="2">
         <v>86000</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
+    <row r="141" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B141" s="2">
         <v>113000</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
+    <row r="142" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B142" s="2">
         <v>54000</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
+    <row r="143" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B143" s="2">
         <v>219000</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
+    <row r="144" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B144" s="2">
         <v>117000</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
+    <row r="145" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B145" s="2">
         <v>798000</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
+    <row r="146" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B146" s="2">
         <v>73000</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
+    <row r="147" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B147" s="2">
         <v>116000</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="4" t="s">
+    <row r="148" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B148" s="2">
         <v>139000</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
+    <row r="149" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B149" s="2">
         <v>55000</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A146" s="4" t="s">
+    <row r="150" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B150" s="2">
         <v>216000</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
+    <row r="151" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B147" s="6">
+      <c r="B151" s="2">
         <v>78000</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="4" t="s">
+    <row r="152" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B152" s="2">
         <v>60000</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="3" t="s">
+    <row r="153" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B149" s="6">
+      <c r="B153" s="2">
         <v>16577000</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="4" t="s">
+    <row r="154" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B154" s="2">
         <v>1411000</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
+    <row r="155" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B151" s="6">
+      <c r="B155" s="2">
         <v>162000</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="s">
+    <row r="156" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B152" s="6">
+      <c r="B156" s="2">
         <v>526000</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+    <row r="157" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B153" s="6">
+      <c r="B157" s="2">
         <v>558000</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="4" t="s">
+    <row r="158" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B154" s="6">
+      <c r="B158" s="2">
         <v>62000</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+    <row r="159" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B155" s="6">
+      <c r="B159" s="2">
         <v>538000</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="4" t="s">
+    <row r="160" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B156" s="6">
+      <c r="B160" s="2">
         <v>1029000</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="4" t="s">
+    <row r="161" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B157" s="6">
+      <c r="B161" s="2">
         <v>195000</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="4" t="s">
+    <row r="162" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B158" s="6">
+      <c r="B162" s="2">
         <v>258000</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
+    <row r="163" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B159" s="6">
+      <c r="B163" s="2">
         <v>2706000</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
+    <row r="164" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B160" s="6">
+      <c r="B164" s="2">
         <v>246000</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
+    <row r="165" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B161" s="6">
+      <c r="B165" s="2">
         <v>137000</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="4" t="s">
+    <row r="166" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B162" s="6">
+      <c r="B166" s="2">
         <v>940000</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="4" t="s">
+    <row r="167" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B163" s="6">
+      <c r="B167" s="2">
         <v>358000</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
+    <row r="168" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B164" s="6">
+      <c r="B168" s="2">
         <v>519000</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
+    <row r="169" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B165" s="6">
+      <c r="B169" s="2">
         <v>1041000</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="4" t="s">
+    <row r="170" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B166" s="6">
+      <c r="B170" s="2">
         <v>163000</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
+    <row r="171" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B167" s="6">
+      <c r="B171" s="2">
         <v>202000</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="4" t="s">
+    <row r="172" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B168" s="6">
+      <c r="B172" s="2">
         <v>473000</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
+    <row r="173" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B169" s="6">
+      <c r="B173" s="2">
         <v>55000</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
+    <row r="174" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B170" s="6">
+      <c r="B174" s="2">
         <v>45000</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+    <row r="175" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B171" s="6">
+      <c r="B175" s="2">
         <v>103000</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="4" t="s">
+    <row r="176" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B172" s="6">
+      <c r="B176" s="2">
         <v>2077000</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+    <row r="177" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B173" s="6">
+      <c r="B177" s="2">
         <v>542000</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="4" t="s">
+    <row r="178" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B174" s="6">
+      <c r="B178" s="2">
         <v>85000</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
+    <row r="179" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B175" s="6">
+      <c r="B179" s="2">
         <v>137000</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="4" t="s">
+    <row r="180" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B176" s="6">
+      <c r="B180" s="2">
         <v>232000</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+    <row r="181" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B177" s="6">
+      <c r="B181" s="2">
         <v>136000</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="4" t="s">
+    <row r="182" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B178" s="6">
+      <c r="B182" s="2">
         <v>520000</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+    <row r="183" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B179" s="6">
+      <c r="B183" s="2">
         <v>328000</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="4" t="s">
+    <row r="184" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B180" s="6">
+      <c r="B184" s="2">
         <v>17000</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="4" t="s">
+    <row r="185" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B181" s="6">
+      <c r="B185" s="2">
         <v>82000</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="4" t="s">
+    <row r="186" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B182" s="6">
+      <c r="B186" s="2">
         <v>37000</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="4" t="s">
+    <row r="187" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B183" s="6">
+      <c r="B187" s="2">
         <v>80000</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="4" t="s">
+    <row r="188" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B184" s="6">
+      <c r="B188" s="2">
         <v>178000</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="4" t="s">
+    <row r="189" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B185" s="6">
+      <c r="B189" s="2">
         <v>401000</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="9" t="s">
+    <row r="191" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B187" s="6">
+      <c r="B191" s="2">
         <v>8012000</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="3" t="s">
+    <row r="192" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B188" s="6">
+      <c r="B192" s="2">
         <v>6693000</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="4" t="s">
+    <row r="193" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B189" s="6">
+      <c r="B193" s="2">
         <v>575000</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="4" t="s">
+    <row r="194" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B190" s="6">
+      <c r="B194" s="2">
         <v>239000</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+    <row r="195" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B191" s="6">
+      <c r="B195" s="2">
         <v>62000</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="4" t="s">
+    <row r="196" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B192" s="6">
+      <c r="B196" s="2">
         <v>2038000</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="4" t="s">
+    <row r="197" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B193" s="6">
+      <c r="B197" s="2">
         <v>515000</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="4" t="s">
+    <row r="198" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B194" s="6">
+      <c r="B198" s="2">
         <v>420000</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="4" t="s">
+    <row r="199" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B195" s="6">
+      <c r="B199" s="2">
         <v>53000</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="4" t="s">
+    <row r="200" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B196" s="6">
+      <c r="B200" s="2">
         <v>36000</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="4" t="s">
+    <row r="201" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B197" s="6">
+      <c r="B201" s="2">
         <v>747000</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="4" t="s">
+    <row r="202" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B198" s="6">
+      <c r="B202" s="2">
         <v>653000</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="4" t="s">
+    <row r="203" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B199" s="6">
+      <c r="B203" s="2">
         <v>787000</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="4" t="s">
+    <row r="204" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B200" s="6">
+      <c r="B204" s="2">
         <v>569000</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="3" t="s">
+    <row r="205" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B201" s="6">
+      <c r="B205" s="2">
         <v>1319000</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A202" s="4" t="s">
+    <row r="206" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B202" s="6">
+      <c r="B206" s="2">
         <v>698000</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="4" t="s">
+    <row r="207" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B203" s="6">
+      <c r="B207" s="2">
         <v>142000</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="4" t="s">
+    <row r="208" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B204" s="6">
+      <c r="B208" s="2">
         <v>105000</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A205" s="4" t="s">
+    <row r="209" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B205" s="6">
+      <c r="B209" s="2">
         <v>249000</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="4" t="s">
+    <row r="210" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B206" s="6">
+      <c r="B210" s="2">
         <v>96000</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="4" t="s">
+    <row r="211" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B207" s="6">
+      <c r="B211" s="2">
         <v>28000</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="9" t="s">
+    <row r="213" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B209" s="6">
+      <c r="B213" s="2">
         <v>2855000</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="3" t="s">
+    <row r="214" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B210" s="6">
+      <c r="B214" s="2">
         <v>199000</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="3" t="s">
+    <row r="215" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B211" s="6">
+      <c r="B215" s="2">
         <v>210000</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="3" t="s">
+    <row r="216" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B212" s="6">
+      <c r="B216" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="3" t="s">
+    <row r="217" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B213" s="6">
+      <c r="B217" s="2">
         <v>436000</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="3" t="s">
+    <row r="218" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B214" s="6">
+      <c r="B218" s="2">
         <v>33000</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A215" s="3" t="s">
+    <row r="219" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B215" s="6">
+      <c r="B219" s="2">
         <v>558000</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A216" s="3" t="s">
+    <row r="220" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B216" s="6">
+      <c r="B220" s="2">
         <v>130000</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="3" t="s">
+    <row r="221" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B217" s="6">
+      <c r="B221" s="2">
         <v>466000</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="3" t="s">
+    <row r="222" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B218" s="6">
+      <c r="B222" s="2">
         <v>400000</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="3" t="s">
+    <row r="223" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B219" s="6">
+      <c r="B223" s="2">
         <v>112000</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="3" t="s">
+    <row r="224" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B220" s="6">
+      <c r="B224" s="2">
         <v>179000</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="3" t="s">
+    <row r="225" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B221" s="6">
+      <c r="B225" s="2">
         <v>31000</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="9" t="s">
+    <row r="227" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B223" s="6">
+      <c r="B227" s="2">
         <v>10404000</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="3" t="s">
+    <row r="228" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B224" s="6">
+      <c r="B228" s="2">
         <v>7241000</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="4" t="s">
+    <row r="229" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B225" s="6">
+      <c r="B229" s="2">
         <v>2102000</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="4" t="s">
+    <row r="230" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B226" s="6">
+      <c r="B230" s="2">
         <v>238000</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="4" t="s">
+    <row r="231" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B227" s="6">
+      <c r="B231" s="2">
         <v>954000</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A228" s="4" t="s">
+    <row r="232" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B228" s="6">
+      <c r="B232" s="2">
         <v>1153000</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="4" t="s">
+    <row r="233" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B229" s="6">
+      <c r="B233" s="2">
         <v>2794000</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="3" t="s">
+    <row r="234" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B230" s="6">
+      <c r="B234" s="2">
         <v>3163000</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="4" t="s">
+    <row r="235" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B231" s="6">
+      <c r="B235" s="2">
         <v>2764000</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="4" t="s">
+    <row r="236" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B232" s="6">
+      <c r="B236" s="2">
         <v>399000</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="5" t="s">
+    <row r="237" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B233" s="6">
+      <c r="B237" s="2">
         <v>179000</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="5" t="s">
+    <row r="238" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B234" s="6">
+      <c r="B238" s="2">
         <v>7000</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="5" t="s">
+    <row r="239" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B235" s="6">
+      <c r="B239" s="2">
         <v>107000</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A236" s="5" t="s">
+    <row r="240" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B236" s="6">
+      <c r="B240" s="2">
         <v>106000</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" s="9" t="s">
+    <row r="242" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B238" s="6">
+      <c r="B242" s="2">
         <v>18325000</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="3" t="s">
+    <row r="243" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B239" s="6">
+      <c r="B243" s="2">
         <v>11228000</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="4" t="s">
+    <row r="244" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B240" s="6">
+      <c r="B244" s="2">
         <v>1610000</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A241" s="4" t="s">
+    <row r="245" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B241" s="6">
+      <c r="B245" s="2">
         <v>1110000</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="4" t="s">
+    <row r="246" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B242" s="6">
+      <c r="B246" s="2">
         <v>1652000</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" s="4" t="s">
+    <row r="247" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B243" s="6">
+      <c r="B247" s="2">
         <v>402000</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A244" s="4" t="s">
+    <row r="248" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B244" s="6">
+      <c r="B248" s="2">
         <v>2845000</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A245" s="4" t="s">
+    <row r="249" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B245" s="6">
+      <c r="B249" s="2">
         <v>1652000</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="4" t="s">
+    <row r="250" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B246" s="6">
+      <c r="B250" s="2">
         <v>597000</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" s="4" t="s">
+    <row r="251" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B247" s="6">
+      <c r="B251" s="2">
         <v>548000</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="4" t="s">
+    <row r="252" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="B248" s="6">
+      <c r="B252" s="2">
         <v>347000</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A249" s="4" t="s">
+    <row r="253" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="B249" s="6">
+      <c r="B253" s="2">
         <v>464000</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="3" t="s">
+    <row r="254" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B250" s="6">
+      <c r="B254" s="2">
         <v>7097000</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" s="4" t="s">
+    <row r="255" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B251" s="6">
+      <c r="B255" s="2">
         <v>188000</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" s="4" t="s">
+    <row r="256" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B252" s="6">
+      <c r="B256" s="2">
         <v>1046000</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="4" t="s">
+    <row r="257" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B253" s="6">
+      <c r="B257" s="2">
         <v>808000</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="4" t="s">
+    <row r="258" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B254" s="6">
+      <c r="B258" s="2">
         <v>304000</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="4" t="s">
+    <row r="259" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B255" s="6">
+      <c r="B259" s="2">
         <v>828000</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" s="4" t="s">
+    <row r="260" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B256" s="6">
+      <c r="B260" s="2">
         <v>1599000</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="4" t="s">
+    <row r="261" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B257" s="6">
+      <c r="B261" s="2">
         <v>1412000</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" s="4" t="s">
+    <row r="262" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B258" s="6">
+      <c r="B262" s="2">
         <v>334000</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" s="4" t="s">
+    <row r="263" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B259" s="6">
+      <c r="B263" s="2">
         <v>577000</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" s="9" t="s">
+    <row r="265" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B261" s="6">
+      <c r="B265" s="2">
         <v>34263000</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="3" t="s">
+    <row r="266" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B262" s="6">
+      <c r="B266" s="2">
         <v>13674000</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" s="4" t="s">
+    <row r="267" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B263" s="6">
+      <c r="B267" s="2">
         <v>8975000</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A264" s="4" t="s">
+    <row r="268" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="B264" s="6">
+      <c r="B268" s="2">
         <v>3851000</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" s="4" t="s">
+    <row r="269" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A269" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B265" s="6">
+      <c r="B269" s="2">
         <v>101000</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A266" s="4" t="s">
+    <row r="270" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B266" s="6">
+      <c r="B270" s="2">
         <v>746000</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" s="3" t="s">
+    <row r="271" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B267" s="6">
+      <c r="B271" s="2">
         <v>20589000</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="4" t="s">
+    <row r="272" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B268" s="6">
+      <c r="B272" s="2">
         <v>6990000</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A269" s="4" t="s">
+    <row r="273" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B269" s="6">
+      <c r="B273" s="2">
         <v>10220000</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" s="5" t="s">
+    <row r="274" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B270" s="6">
+      <c r="B274" s="2">
         <v>1611000</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="5" t="s">
+    <row r="275" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B271" s="6">
+      <c r="B275" s="2">
         <v>897000</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" s="5" t="s">
+    <row r="276" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B272" s="6">
+      <c r="B276" s="2">
         <v>135000</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" s="5" t="s">
+    <row r="277" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B273" s="6">
+      <c r="B277" s="2">
         <v>133000</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" s="5" t="s">
+    <row r="278" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B274" s="6">
+      <c r="B278" s="2">
         <v>297000</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="5" t="s">
+    <row r="279" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B275" s="6">
+      <c r="B279" s="2">
         <v>1603000</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" s="5" t="s">
+    <row r="280" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B276" s="6">
+      <c r="B280" s="2">
         <v>1495000</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="5" t="s">
+    <row r="281" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B277" s="6">
+      <c r="B281" s="2">
         <v>1417000</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" s="5" t="s">
+    <row r="282" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B278" s="6">
+      <c r="B282" s="2">
         <v>1786000</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A279" s="5" t="s">
+    <row r="283" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B279" s="6">
+      <c r="B283" s="2">
         <v>846000</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="4" t="s">
+    <row r="284" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="B280" s="6">
+      <c r="B284" s="2">
         <v>3379000</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" s="5" t="s">
+    <row r="285" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B281" s="6">
+      <c r="B285" s="2">
         <v>1553000</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A282" s="5" t="s">
+    <row r="286" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B282" s="6">
+      <c r="B286" s="2">
         <v>127000</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" s="5" t="s">
+    <row r="287" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B283" s="6">
+      <c r="B287" s="2">
         <v>138000</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" s="5" t="s">
+    <row r="288" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A288" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B284" s="6">
+      <c r="B288" s="2">
         <v>1561000</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" s="9" t="s">
+    <row r="290" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="B286" s="6">
+      <c r="B290" s="2">
         <v>14193000</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" s="3" t="s">
+    <row r="291" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B287" s="6">
+      <c r="B291" s="2">
         <v>3241000</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A288" s="4" t="s">
+    <row r="292" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="B288" s="6">
+      <c r="B292" s="2">
         <v>857000</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A289" s="4" t="s">
+    <row r="293" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A293" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="B289" s="6">
+      <c r="B293" s="2">
         <v>364000</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="4" t="s">
+    <row r="294" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A294" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B290" s="6">
+      <c r="B294" s="2">
         <v>33000</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A291" s="4" t="s">
+    <row r="295" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="B291" s="6">
+      <c r="B295" s="2">
         <v>1988000</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" s="3" t="s">
+    <row r="296" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B292" s="6">
+      <c r="B296" s="2">
         <v>10952000</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" s="4" t="s">
+    <row r="297" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="B293" s="6">
+      <c r="B297" s="2">
         <v>1592000</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" s="5" t="s">
+    <row r="298" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="B294" s="6">
+      <c r="B298" s="2">
         <v>1488000</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A295" s="5" t="s">
+    <row r="299" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B295" s="6">
+      <c r="B299" s="2">
         <v>104000</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A296" s="4" t="s">
+    <row r="300" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A300" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B296" s="6">
+      <c r="B300" s="2">
         <v>9360000</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A297" s="5" t="s">
+    <row r="301" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A301" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B297" s="6">
+      <c r="B301" s="2">
         <v>9134000</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" s="5" t="s">
+    <row r="302" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="B298" s="6">
+      <c r="B302" s="2">
         <v>226000</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A300" s="9" t="s">
+    <row r="304" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B300" s="6">
+      <c r="B304" s="2">
         <v>7320000</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A301" s="3" t="s">
+    <row r="305" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B301" s="6">
+      <c r="B305" s="2">
         <v>6596000</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A302" s="4" t="s">
+    <row r="306" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B302" s="6">
+      <c r="B306" s="2">
         <v>2051000</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A303" s="5" t="s">
+    <row r="307" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="B303" s="6">
+      <c r="B307" s="2">
         <v>1205000</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A304" s="5" t="s">
+    <row r="308" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="B304" s="6">
+      <c r="B308" s="2">
         <v>168000</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A305" s="5" t="s">
+    <row r="309" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B305" s="6">
+      <c r="B309" s="2">
         <v>134000</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A306" s="5" t="s">
+    <row r="310" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B306" s="6">
+      <c r="B310" s="2">
         <v>322000</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A307" s="5" t="s">
+    <row r="311" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B307" s="6">
+      <c r="B311" s="2">
         <v>218000</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="5" t="s">
+    <row r="312" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A312" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B308" s="6">
+      <c r="B312" s="2">
         <v>5000</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="4" t="s">
+    <row r="313" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="B309" s="6">
+      <c r="B313" s="2">
         <v>2481000</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A310" s="5" t="s">
+    <row r="314" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B310" s="6">
+      <c r="B314" s="2">
         <v>134000</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="5" t="s">
+    <row r="315" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A315" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B311" s="6">
+      <c r="B315" s="2">
         <v>982000</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="5" t="s">
+    <row r="316" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="B312" s="6">
+      <c r="B316" s="2">
         <v>541000</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A313" s="5" t="s">
+    <row r="317" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A317" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="B313" s="6">
+      <c r="B317" s="2">
         <v>286000</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A314" s="5" t="s">
+    <row r="318" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B314" s="6">
+      <c r="B318" s="2">
         <v>149000</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A315" s="5" t="s">
+    <row r="319" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B315" s="6">
+      <c r="B319" s="2">
         <v>389000</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A316" s="4" t="s">
+    <row r="320" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B316" s="6">
+      <c r="B320" s="2">
         <v>2064000</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A317" s="5" t="s">
+    <row r="321" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B317" s="6">
+      <c r="B321" s="2">
         <v>1088000</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A318" s="5" t="s">
+    <row r="322" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B318" s="6">
+      <c r="B322" s="2">
         <v>754000</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A319" s="5" t="s">
+    <row r="323" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="B319" s="6">
+      <c r="B323" s="2">
         <v>58000</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A320" s="5" t="s">
+    <row r="324" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B320" s="6">
+      <c r="B324" s="2">
         <v>164000</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A321" s="3" t="s">
+    <row r="325" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B321" s="6">
+      <c r="B325" s="2">
         <v>724000</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A323" s="9" t="s">
+    <row r="327" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B323" s="6">
+      <c r="B327" s="2">
         <v>6857000</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A324" s="3" t="s">
+    <row r="328" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B324" s="6">
+      <c r="B328" s="2">
         <v>1082000</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A325" s="3" t="s">
+    <row r="329" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B325" s="6">
+      <c r="B329" s="2">
         <v>302000</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A326" s="3" t="s">
+    <row r="330" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B326" s="6">
+      <c r="B330" s="2">
         <v>106000</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A327" s="3" t="s">
+    <row r="331" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B327" s="6">
+      <c r="B331" s="2">
         <v>2739000</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A328" s="3" t="s">
+    <row r="332" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A332" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B328" s="6">
+      <c r="B332" s="2">
         <v>995000</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A329" s="3" t="s">
+    <row r="333" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A333" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B329" s="6">
+      <c r="B333" s="2">
         <v>248000</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A330" s="3" t="s">
+    <row r="334" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A334" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B330" s="6">
+      <c r="B334" s="2">
         <v>529000</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A331" s="3" t="s">
+    <row r="335" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A335" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B331" s="6">
+      <c r="B335" s="2">
         <v>857000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added full listing of all professionals, because "face boss"
</commit_message>
<xml_diff>
--- a/Data/03_ProportionData/USIndustryEmploymentData2016.xlsx
+++ b/Data/03_ProportionData/USIndustryEmploymentData2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40740" yWindow="460" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B335"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>

</xml_diff>